<commit_message>
Updated spreadsheet column names
</commit_message>
<xml_diff>
--- a/cmip5/vocab-mappings/ocean/ocean-key-properties.xlsx
+++ b/cmip5/vocab-mappings/ocean/ocean-key-properties.xlsx
@@ -1,18 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27224"/>
   <workbookPr date1904="1"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macg/dev/esdoc/repos/esdoc-docs/cmip5/vocab-mappings/ocean/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <calcPr calcId="0" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="40">
   <si>
     <t>Table 1</t>
   </si>
@@ -23,9 +38,6 @@
     <t>cmip5-component-property</t>
   </si>
   <si>
-    <t>cmip6-detail-property-id</t>
-  </si>
-  <si>
     <t>mapping-qc-status</t>
   </si>
   <si>
@@ -132,16 +144,16 @@
   </si>
   <si>
     <t>Time Stepping Framework &gt; Tracers</t>
+  </si>
+  <si>
+    <t>cmip6-id</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -153,7 +165,7 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Helvetica"/>
@@ -228,68 +240,125 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
   <cellXfs count="10">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
-      <rgbColor rgb="ff3f3f3f"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFBDC0BF"/>
+      <rgbColor rgb="FFA5A5A5"/>
+      <rgbColor rgb="FF3F3F3F"/>
+      <rgbColor rgb="000000D4"/>
+      <rgbColor rgb="00FCF305"/>
+      <rgbColor rgb="00F20884"/>
+      <rgbColor rgb="0000ABEA"/>
+      <rgbColor rgb="00900000"/>
+      <rgbColor rgb="00006411"/>
+      <rgbColor rgb="00000090"/>
+      <rgbColor rgb="0090713A"/>
+      <rgbColor rgb="004600A5"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0063AAFE"/>
+      <rgbColor rgb="00DD2D32"/>
+      <rgbColor rgb="00FFF58C"/>
+      <rgbColor rgb="004EE257"/>
+      <rgbColor rgb="006711FF"/>
+      <rgbColor rgb="00FEA746"/>
+      <rgbColor rgb="00865357"/>
+      <rgbColor rgb="00A2BD90"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Blank">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Blank">
   <a:themeElements>
     <a:clrScheme name="Blank">
       <a:dk1>
@@ -415,7 +484,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -424,7 +493,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -433,7 +502,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
               </a:srgbClr>
@@ -497,8 +566,8 @@
     <a:spDef>
       <a:spPr>
         <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+          <a:srcRect/>
           <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
         </a:blipFill>
         <a:ln w="12700" cap="flat">
@@ -506,7 +575,7 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+          <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
             <a:srgbClr val="000000">
               <a:alpha val="50000"/>
             </a:srgbClr>
@@ -514,7 +583,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -533,7 +602,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1200" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -541,7 +610,7 @@
               <a:srgbClr val="FFFFFF"/>
             </a:solidFill>
             <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+              <a:outerShdw blurRad="25400" dist="23998" dir="2700000" rotWithShape="0">
                 <a:srgbClr val="000000">
                   <a:alpha val="31034"/>
                 </a:srgbClr>
@@ -569,7 +638,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -595,7 +664,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -621,7 +690,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -647,7 +716,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -673,7 +742,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -699,7 +768,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -725,7 +794,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -751,7 +820,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -777,7 +846,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -790,9 +859,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -809,7 +884,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -828,7 +903,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -854,7 +929,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -880,7 +955,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -906,7 +981,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -932,7 +1007,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -958,7 +1033,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -984,7 +1059,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1010,7 +1085,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1036,7 +1111,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,7 +1137,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1075,9 +1150,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1091,7 +1172,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1110,7 +1191,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1140,7 +1221,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1166,7 +1247,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1192,7 +1273,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1218,7 +1299,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1244,7 +1325,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1270,7 +1351,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1296,7 +1377,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1322,7 +1403,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1348,7 +1429,7 @@
           <a:buFontTx/>
           <a:buNone/>
           <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1361,509 +1442,518 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A2:D44"/>
+  <dimension ref="A1:IV44"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.33333" defaultRowHeight="18" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.33203125" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="17.6719" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="58" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="16.3516" style="1" customWidth="1"/>
-    <col min="5" max="256" width="8.35156" style="1" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" style="1" customWidth="1"/>
+    <col min="5" max="256" width="8.33203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="28" customHeight="1">
-      <c r="A1" t="s" s="2">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-    </row>
-    <row r="2" ht="20.55" customHeight="1">
-      <c r="A2" t="s" s="3">
+    <row r="1" spans="1:4" ht="28" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s" s="3">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" t="s" s="3">
+      <c r="C2" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D2" t="s" s="3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" ht="20.55" customHeight="1">
-      <c r="A3" t="s" s="4">
+    </row>
+    <row r="3" spans="1:4" ht="20.5" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s" s="5">
+      <c r="C3" s="4"/>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="6"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" ht="20.35" customHeight="1">
-      <c r="A4" s="7"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="9"/>
-    </row>
-    <row r="5" ht="20.35" customHeight="1">
-      <c r="A5" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s" s="8">
+      <c r="C5" s="7"/>
+      <c r="D5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" ht="20.35" customHeight="1">
-      <c r="A6" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s" s="8">
+      <c r="C6" s="7"/>
+      <c r="D6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="6"/>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+    </row>
+    <row r="8" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" ht="20.35" customHeight="1">
-      <c r="A7" s="7"/>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-    </row>
-    <row r="8" ht="20.35" customHeight="1">
-      <c r="A8" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s" s="8">
+      <c r="C8" s="7"/>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" ht="20.35" customHeight="1">
-      <c r="A9" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B9" t="s" s="8">
+      <c r="C9" s="7"/>
+      <c r="D9" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" ht="20.35" customHeight="1">
-      <c r="A10" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s" s="8">
+      <c r="C10" s="7"/>
+      <c r="D10" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="6"/>
+      <c r="B11" s="7"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="8"/>
-      <c r="D10" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" ht="20.35" customHeight="1">
-      <c r="A11" s="7"/>
-      <c r="B11" s="8"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" ht="20.35" customHeight="1">
-      <c r="A12" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B12" t="s" s="8">
+      <c r="C12" s="7"/>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="6"/>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" ht="20.35" customHeight="1">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" ht="20.35" customHeight="1">
-      <c r="A14" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B14" t="s" s="8">
+      <c r="C14" s="7"/>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="6"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" ht="20.35" customHeight="1">
-      <c r="A15" s="7"/>
-      <c r="B15" s="8"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-    </row>
-    <row r="16" ht="20.35" customHeight="1">
-      <c r="A16" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B16" t="s" s="8">
+      <c r="C16" s="7"/>
+      <c r="D16" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" ht="20.35" customHeight="1">
-      <c r="A17" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B17" t="s" s="8">
+      <c r="C17" s="7"/>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="6"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" ht="20.35" customHeight="1">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="9"/>
-    </row>
-    <row r="19" ht="20.35" customHeight="1">
-      <c r="A19" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B19" t="s" s="8">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" ht="20.35" customHeight="1">
-      <c r="A20" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B20" t="s" s="8">
+      <c r="C20" s="7"/>
+      <c r="D20" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" ht="20.35" customHeight="1">
-      <c r="A21" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B21" t="s" s="8">
+      <c r="C21" s="7"/>
+      <c r="D21" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" ht="20.35" customHeight="1">
-      <c r="A22" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B22" t="s" s="8">
+      <c r="C22" s="7"/>
+      <c r="D22" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" ht="20.35" customHeight="1">
-      <c r="A23" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B23" t="s" s="8">
+      <c r="C23" s="7"/>
+      <c r="D23" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" ht="20.35" customHeight="1">
-      <c r="A24" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B24" t="s" s="8">
+      <c r="C24" s="7"/>
+      <c r="D24" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" ht="20.35" customHeight="1">
-      <c r="A25" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B25" t="s" s="8">
+      <c r="C25" s="7"/>
+      <c r="D25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B26" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" ht="20.35" customHeight="1">
-      <c r="A26" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B26" t="s" s="8">
+      <c r="C26" s="7"/>
+      <c r="D26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="8"/>
-      <c r="D26" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" ht="20.35" customHeight="1">
-      <c r="A27" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B27" t="s" s="8">
+      <c r="C27" s="7"/>
+      <c r="D27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B28" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" ht="20.35" customHeight="1">
-      <c r="A28" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B28" t="s" s="8">
+      <c r="C28" s="7"/>
+      <c r="D28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B29" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" ht="20.35" customHeight="1">
-      <c r="A29" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B29" t="s" s="8">
+      <c r="C29" s="7"/>
+      <c r="D29" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" ht="20.35" customHeight="1">
-      <c r="A30" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B30" t="s" s="8">
+      <c r="C30" s="7"/>
+      <c r="D30" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="8"/>
-      <c r="D30" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" ht="20.35" customHeight="1">
-      <c r="A31" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B31" t="s" s="8">
+      <c r="C31" s="7"/>
+      <c r="D31" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" ht="20.35" customHeight="1">
-      <c r="A32" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B32" t="s" s="8">
+      <c r="C32" s="7"/>
+      <c r="D32" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="8"/>
-      <c r="D32" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" ht="20.35" customHeight="1">
-      <c r="A33" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B33" t="s" s="8">
+      <c r="C33" s="7"/>
+      <c r="D33" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="6"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" ht="20.35" customHeight="1">
-      <c r="A34" s="7"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="9"/>
-    </row>
-    <row r="35" ht="20.35" customHeight="1">
-      <c r="A35" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B35" t="s" s="8">
+      <c r="C35" s="7"/>
+      <c r="D35" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="8"/>
-      <c r="D35" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" ht="20.35" customHeight="1">
-      <c r="A36" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B36" t="s" s="8">
+      <c r="C36" s="7"/>
+      <c r="D36" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="8"/>
-      <c r="D36" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" ht="20.35" customHeight="1">
-      <c r="A37" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B37" t="s" s="8">
+      <c r="C37" s="7"/>
+      <c r="D37" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B38" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="8"/>
-      <c r="D37" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" ht="20.35" customHeight="1">
-      <c r="A38" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B38" t="s" s="8">
+      <c r="C38" s="7"/>
+      <c r="D38" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B39" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="8"/>
-      <c r="D38" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" ht="20.35" customHeight="1">
-      <c r="A39" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B39" t="s" s="8">
+      <c r="C39" s="7"/>
+      <c r="D39" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="6"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B41" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="8"/>
-      <c r="D39" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" ht="20.35" customHeight="1">
-      <c r="A40" s="7"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="9"/>
-    </row>
-    <row r="41" ht="20.35" customHeight="1">
-      <c r="A41" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B41" t="s" s="8">
+      <c r="C41" s="7"/>
+      <c r="D41" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B42" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="8"/>
-      <c r="D41" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" ht="20.35" customHeight="1">
-      <c r="A42" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B42" t="s" s="8">
+      <c r="C42" s="7"/>
+      <c r="D42" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="C42" s="8"/>
-      <c r="D42" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" ht="20.35" customHeight="1">
-      <c r="A43" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B43" t="s" s="8">
+      <c r="C43" s="7"/>
+      <c r="D43" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B44" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" ht="20.35" customHeight="1">
-      <c r="A44" t="s" s="7">
-        <v>5</v>
-      </c>
-      <c r="B44" t="s" s="8">
-        <v>39</v>
-      </c>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9">
+      <c r="C44" s="7"/>
+      <c r="D44" s="8">
         <v>0</v>
       </c>
     </row>
@@ -1872,7 +1962,7 @@
     <mergeCell ref="A1:D1"/>
   </mergeCells>
   <pageMargins left="1" right="1" top="1" bottom="1" header="0.25" footer="0.25"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>